<commit_message>
excel reading is workig
excel get read properly . time to fill it up
</commit_message>
<xml_diff>
--- a/Appartment_database_template.xlsx
+++ b/Appartment_database_template.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penoelothibeaud/Desktop/projet/Software engineering/Personal project/Appartment condition check/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penoelothibeaud/Desktop/projet/Software engineering/Personal project/Appartment condition check/App_search_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF50B1E-DDFE-A64C-AE75-16813C7C8712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA90D1-2C42-CD4D-980C-95B00CF7D46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16300" xr2:uid="{4330DD11-BDF7-F443-8572-BFA9AE275412}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{4330DD11-BDF7-F443-8572-BFA9AE275412}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Address</t>
   </si>
@@ -170,6 +169,12 @@
   </si>
   <si>
     <t>montreal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity_to </t>
+  </si>
+  <si>
+    <t>Sir George Williams Campus, Montreal, Quebec H3G 1M8, Canada</t>
   </si>
 </sst>
 </file>
@@ -472,6 +477,60 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,12 +555,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,54 +565,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -983,9 +988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566F71E9-EAC0-3C40-BC9C-7CFC1F725265}">
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="175" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,79 +1021,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="35" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="31" t="s">
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="32" t="s">
+      <c r="X1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Y1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="29"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="47"/>
     </row>
     <row r="2" spans="1:29" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="53" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="44" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
       <c r="M2" s="33" t="s">
         <v>15</v>
       </c>
@@ -1107,39 +1112,39 @@
       <c r="R2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="27" t="s">
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="38" t="s">
+      <c r="AB2" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AC2" s="49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="15" t="s">
         <v>27</v>
       </c>
@@ -1164,17 +1169,17 @@
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="34"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
       <c r="W3" s="3"/>
       <c r="X3" s="17"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="18"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="32"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="50"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -1271,18 +1276,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AA2:AA3"/>
@@ -1299,6 +1292,18 @@
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1309,16 +1314,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB89B5D-C0D8-0949-80EC-8171E8E9E8EB}">
-  <dimension ref="A2:B8"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="21.1640625" customWidth="1"/>
   </cols>
@@ -1379,6 +1384,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
still can slide the price
fixed and tested a bunch of bugs
</commit_message>
<xml_diff>
--- a/Appartment_database_template.xlsx
+++ b/Appartment_database_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penoelothibeaud/Desktop/projet/Software engineering/Personal project/Appartment condition check/App_search_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA193FF-B557-F646-ACA5-B1A61563B724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AA4B33-A4C9-3842-9C09-C3346ED2D049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{4330DD11-BDF7-F443-8572-BFA9AE275412}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{4330DD11-BDF7-F443-8572-BFA9AE275412}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Address</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Sir George Williams Campus, Montreal, Quebec H3G 1M8, Canada</t>
+  </si>
+  <si>
+    <t>min price</t>
   </si>
 </sst>
 </file>
@@ -477,6 +480,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,12 +546,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,42 +568,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1021,79 +1024,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="51" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="49" t="s">
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="50" t="s">
+      <c r="X1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="49" t="s">
+      <c r="Y1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="Z1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="45" t="s">
+      <c r="AA1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="47"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="29"/>
     </row>
     <row r="2" spans="1:29" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="41" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="30" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="32"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46"/>
       <c r="M2" s="33" t="s">
         <v>15</v>
       </c>
@@ -1112,39 +1115,39 @@
       <c r="R2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="43" t="s">
+      <c r="S2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="43" t="s">
+      <c r="U2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="V2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="45" t="s">
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="54" t="s">
+      <c r="AB2" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="49" t="s">
+      <c r="AC2" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="15" t="s">
         <v>27</v>
       </c>
@@ -1169,17 +1172,17 @@
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="34"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
       <c r="W3" s="3"/>
       <c r="X3" s="17"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="18"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="50"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -1276,6 +1279,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AA2:AA3"/>
@@ -1292,18 +1307,6 @@
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:R1"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1314,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB89B5D-C0D8-0949-80EC-8171E8E9E8EB}">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="207" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,15 +1365,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1378,17 +1381,25 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>